<commit_message>
New Eyetracking Tagging and EEG Timestamps
</commit_message>
<xml_diff>
--- a/Stimuli/DRM_Setlists.xlsx
+++ b/Stimuli/DRM_Setlists.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\CEPSW-Psychology BC Lab\Tess\Tobii\Noarlunga Project\Stimuli\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{708CC00F-DBEF-4040-80F0-4874FF43B481}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{953A9670-F932-4C92-9C60-7AE34B958A55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{53261134-AD4F-41FC-96F7-DDA86AC5C7FC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="484">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="485">
   <si>
     <t xml:space="preserve">Encoding Phase Lists </t>
   </si>
@@ -1486,6 +1486,9 @@
   </si>
   <si>
     <t>Monarch</t>
+  </si>
+  <si>
+    <t>Fur</t>
   </si>
 </sst>
 </file>
@@ -1880,7 +1883,7 @@
   <dimension ref="A1:X54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="T7" sqref="T7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2320,7 +2323,7 @@
         <v>139</v>
       </c>
       <c r="T7" t="s">
-        <v>140</v>
+        <v>484</v>
       </c>
       <c r="U7" t="s">
         <v>141</v>

</xml_diff>